<commit_message>
CORS errors and critical HBD transfer bug corrected
</commit_message>
<xml_diff>
--- a/TestTable.xlsx
+++ b/TestTable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>Guest checkout</t>
   </si>
@@ -66,16 +66,26 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>NOK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,8 +111,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,14 +397,15 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="4" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
     <col min="6" max="6" width="25.7109375" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" customWidth="1"/>
@@ -437,6 +449,9 @@
       <c r="C2" t="s">
         <v>13</v>
       </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -445,6 +460,15 @@
       <c r="B3" t="s">
         <v>13</v>
       </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -453,6 +477,12 @@
       <c r="B4" t="s">
         <v>13</v>
       </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -461,6 +491,15 @@
       <c r="B5" t="s">
         <v>13</v>
       </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -469,8 +508,15 @@
       <c r="B6" t="s">
         <v>13</v>
       </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>